<commit_message>
Nearly finished dead code
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\SplCompiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0EB0DA-2BD5-445E-80A3-71B8E392D995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9DECA-973F-42C5-807A-ED4609D733CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="77">
   <si>
     <t>Test</t>
   </si>
@@ -227,9 +227,6 @@
     <t>Fix do while shift reduce if change statement_list to code</t>
   </si>
   <si>
-    <t>Remves and warns</t>
-  </si>
-  <si>
     <t>Cast will remove negative so is valid even if stupid…</t>
   </si>
   <si>
@@ -239,9 +236,6 @@
     <t>Error</t>
   </si>
   <si>
-    <t>Loop Unrolling</t>
-  </si>
-  <si>
     <t>Dead store</t>
   </si>
   <si>
@@ -252,6 +246,21 @@
   </si>
   <si>
     <t>In lex, imidiately exits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Me </t>
+  </si>
+  <si>
+    <t>Dead code</t>
+  </si>
+  <si>
+    <t>Removes and warns</t>
+  </si>
+  <si>
+    <t>Needs testing. Should work.</t>
+  </si>
+  <si>
+    <t>Implement constant variables i.e. evaluate variable usage when determing constants (extra hard)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -307,6 +316,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,7 +711,7 @@
         <v>55</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -717,7 +728,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -898,7 +909,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -963,10 +974,10 @@
         <v>59</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1000,7 +1011,7 @@
         <v>42</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,15 +1043,17 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1050,25 +1063,44 @@
         <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
+      <c r="C28" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on test programs
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B9DECA-973F-42C5-807A-ED4609D733CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FEF12A-E988-4171-AB07-9B37AF82865F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Test</t>
   </si>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,19 +1073,19 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Getting there still. Readme is nearly there. Code is okay and nearly there just so much to do
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\LanguagesAndCompilers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FEF12A-E988-4171-AB07-9B37AF82865F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA87CB2-8AD0-4A49-8927-92C03019795B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
+    <workbookView xWindow="-60110" yWindow="-19380" windowWidth="21820" windowHeight="38020" xr2:uid="{50EF48C9-6323-418F-8AB0-BA98C6E84C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="80">
   <si>
     <t>Test</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Implement constant variables i.e. evaluate variable usage when determing constants (extra hard)</t>
+  </si>
+  <si>
+    <t>Line numbers</t>
+  </si>
+  <si>
+    <t>Fix usage in loops…</t>
+  </si>
+  <si>
+    <t>Remove dead declarations…</t>
   </si>
 </sst>
 </file>
@@ -276,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +304,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -308,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -318,6 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075A21D6-570E-47A5-875C-908BD7B48656}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,6 +1118,21 @@
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
     </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>